<commit_message>
different entries for software, depending on whether they have a homepage
</commit_message>
<xml_diff>
--- a/data-raw/works.xlsx
+++ b/data-raw/works.xlsx
@@ -14,57 +14,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="145">
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
   <si>
     <t>Authors</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>description</t>
+    <t>url</t>
   </si>
   <si>
     <t>Title</t>
   </si>
   <si>
-    <t>url</t>
+    <t>url_short</t>
+  </si>
+  <si>
+    <t>started</t>
   </si>
   <si>
     <t>Publication</t>
   </si>
   <si>
-    <t>url_short</t>
-  </si>
-  <si>
-    <t>started</t>
+    <t>last_updated</t>
   </si>
   <si>
     <t>Volume</t>
   </si>
   <si>
+    <t>finished</t>
+  </si>
+  <si>
     <t>Number</t>
   </si>
   <si>
-    <t>last_updated</t>
+    <t>On Polytopes and Lattice-Point Enumeration</t>
   </si>
   <si>
     <t>Pages</t>
   </si>
   <si>
-    <t>finished</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
+    <t>Completing KF-SPLS with Ryser</t>
+  </si>
+  <si>
     <t>Publisher</t>
   </si>
   <si>
-    <t>On Polytopes and Lattice-Point Enumeration</t>
-  </si>
-  <si>
-    <t>Completing KF-SPLS with Ryser</t>
+    <t>Notes on Ehrhart Theory, including examples in Polymake.</t>
   </si>
   <si>
     <t xml:space="preserve">Davis, Sean; Henderson, Matthew; Smith, Andrew; </t>
@@ -76,9 +79,6 @@
     <t>Proceedings of the 9th Python in Science Conference</t>
   </si>
   <si>
-    <t>Notes on Ehrhart Theory, including examples in Polymake.</t>
-  </si>
-  <si>
     <t>An [IPython][ipython] notebook demonstrating some ideas about completing KF-SPLS using the [Ryser][ryserhome] package for partial latin square completion.</t>
   </si>
   <si>
@@ -112,19 +112,22 @@
     <t>https://nbviewer.jupyter.org/gist/MHenderson/5902080</t>
   </si>
   <si>
+    <t>On the Completability of Wing-Form Partial Latin Squares</t>
+  </si>
+  <si>
+    <t>Completable, bound, untethered KF-SPLS of even order are characterised.</t>
+  </si>
+  <si>
+    <t>https://gitlab.com/MHenderson1/notes/blob/master/13_06_28_wingform.pdf</t>
+  </si>
+  <si>
     <t>Springer</t>
   </si>
   <si>
     <t>https://doi.org/10.1007/978-3-642-04211-9_1</t>
   </si>
   <si>
-    <t>On the Completability of Wing-Form Partial Latin Squares</t>
-  </si>
-  <si>
-    <t>Completable, bound, untethered KF-SPLS of even order are characterised.</t>
-  </si>
-  <si>
-    <t>https://gitlab.com/MHenderson1/notes/blob/master/13_06_28_wingform.pdf</t>
+    <t>http://bit.ly/2YIm0U8</t>
   </si>
   <si>
     <t>Collaborative Development of System Architecture-a Tool for Coping with Inconsistency.</t>
@@ -145,13 +148,16 @@
     <t>https://nbviewer.jupyter.org/gist/MHenderson/6279740</t>
   </si>
   <si>
-    <t>http://bit.ly/2YIm0U8</t>
+    <t>Some Observations on the Intricacy of Partial Latin Square Completion</t>
+  </si>
+  <si>
+    <t>Some ideas about the intricacy of completing partial latin squares.</t>
   </si>
   <si>
     <t xml:space="preserve">Henderson, Matthew; Shawe-Taylor, John; Žerovnik, Janez; </t>
   </si>
   <si>
-    <t>Mixture of vector experts</t>
+    <t>Mixture of Vector Experts</t>
   </si>
   <si>
     <t>International Conference on Algorithmic Learning Theory</t>
@@ -160,94 +166,100 @@
     <t>386-398</t>
   </si>
   <si>
-    <t>Some Observations on the Intricacy of Partial Latin Square Completion</t>
-  </si>
-  <si>
-    <t>Some ideas about the intricacy of completing partial latin squares.</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1007/11564089_30</t>
   </si>
   <si>
+    <t>https://gitlab.com/MHenderson1/notes/blob/master/12_09_15_intricacy.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Henderson, Matthew James; </t>
+  </si>
+  <si>
+    <t>Embedding symmetric latin squares and edge-coloured graphs</t>
+  </si>
+  <si>
+    <t>http://bit.ly/2snV3sH</t>
+  </si>
+  <si>
+    <t>University of Reading</t>
+  </si>
+  <si>
+    <t>https://ethos.bl.uk/OrderDetails.do?uin=uk.bl.ethos.485356</t>
+  </si>
+  <si>
     <t>Processing GPS Data in Python</t>
   </si>
   <si>
     <t>An [IPython][ipython] notebook presenting a statistical investigation, based on GPS data, into anomalous driving patterns among a fleet of delivery trucks</t>
   </si>
   <si>
-    <t>https://gitlab.com/MHenderson1/notes/blob/master/12_09_15_intricacy.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Henderson, Matthew James; </t>
-  </si>
-  <si>
-    <t>Embedding symmetric latin squares and edge-coloured graphs</t>
-  </si>
-  <si>
-    <t>University of Reading</t>
-  </si>
-  <si>
-    <t>https://mjh-phd.netlify.com/</t>
-  </si>
-  <si>
-    <t>http://bit.ly/2snV3sH</t>
+    <t>On the Completability of Kite-Form Partial Latin Squares</t>
+  </si>
+  <si>
+    <t>Characterising the completable bound, untethered KF-SPLS of even order.</t>
+  </si>
+  <si>
+    <t>https://gitlab.com/MHenderson1/notes/blob/master/12_06_20_kiteform.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Henderson, MJ; Hilton, AJW; </t>
+  </si>
+  <si>
+    <t>Completing An Edge-Colouring of $ K_ {2m} $ with $ K_r $ and Independent Edges Precoloured</t>
+  </si>
+  <si>
+    <t>Journal of the London Mathematical Society</t>
+  </si>
+  <si>
+    <t>545-566</t>
+  </si>
+  <si>
+    <t>Cambridge University Press</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1112/s0024610704005526</t>
+  </si>
+  <si>
+    <t>http://bit.ly/2rIHjJ6</t>
+  </si>
+  <si>
+    <t>On Pandiagonal Strongly-Symmetric Self-Orthogonal Diagonal Latin Squares</t>
+  </si>
+  <si>
+    <t>Describing the discovery of a PSSSODLS of order 9.</t>
   </si>
   <si>
     <t>Modelling Sudoku Puzzles in Python</t>
   </si>
   <si>
-    <t xml:space="preserve">Henderson, MJ; Hilton, AJW; </t>
-  </si>
-  <si>
     <t>An updated version of {% cite davis7modeling –file mh2 %} as an IPython notebook.</t>
   </si>
   <si>
     <t>https://nbviewer.jupyter.org/gist/MHenderson/6416294</t>
   </si>
   <si>
-    <t>Completing An Edge-Colouring of $ K_ {2m} $ with $ K_r $ and Independent Edges Precoloured</t>
-  </si>
-  <si>
-    <t>Journal of the London Mathematical Society</t>
-  </si>
-  <si>
-    <t>545-566</t>
-  </si>
-  <si>
-    <t>On the Completability of Kite-Form Partial Latin Squares</t>
-  </si>
-  <si>
-    <t>Characterising the completable bound, untethered KF-SPLS of even order.</t>
-  </si>
-  <si>
-    <t>Cambridge University Press</t>
-  </si>
-  <si>
-    <t>https://gitlab.com/MHenderson1/notes/blob/master/12_06_20_kiteform.pdf</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1112/s0024610704005526</t>
+    <t>https://gitlab.com/MHenderson1/notes/blob/master/12_04_16_psssodls.pdf</t>
+  </si>
+  <si>
+    <t>http://bit.ly/2PKgsEq</t>
   </si>
   <si>
     <t>Speech Annotation in Python Using Regular Expressions</t>
   </si>
   <si>
-    <t>http://bit.ly/2rIHjJ6</t>
-  </si>
-  <si>
     <t>An IPython notebook which illustrates some basic ideas about annotating a corpus of novels using regular expressions.</t>
   </si>
   <si>
     <t>https://nbviewer.jupyter.org/gist/MHenderson/6052936</t>
   </si>
   <si>
-    <t>On Pandiagonal Strongly-Symmetric Self-Orthogonal Diagonal Latin Squares</t>
-  </si>
-  <si>
-    <t>Describing the discovery of a PSSSODLS of order 9.</t>
-  </si>
-  <si>
-    <t>https://gitlab.com/MHenderson1/notes/blob/master/12_04_16_psssodls.pdf</t>
+    <t>Constraint Modelling of Pandiagonal Strongly-Symmetric Self-Orthogonal Diagonal Latin Squares</t>
+  </si>
+  <si>
+    <t>Using Essence', Savile Row and Minion to model PSSSODLS.</t>
+  </si>
+  <si>
+    <t>https://gitlab.com/MHenderson1/notes/blob/master/11_12_08_constraint_psssodls.pdf</t>
   </si>
   <si>
     <t>List-colouring in Python with Vizing</t>
@@ -257,18 +269,6 @@
   </si>
   <si>
     <t>https://nbviewer.jupyter.org/gist/MHenderson/5857920</t>
-  </si>
-  <si>
-    <t>http://bit.ly/2PKgsEq</t>
-  </si>
-  <si>
-    <t>Constraint Modelling of Pandiagonal Strongly-Symmetric Self-Orthogonal Diagonal Latin Squares</t>
-  </si>
-  <si>
-    <t>Using Essence', Savile Row and Minion to model PSSSODLS.</t>
-  </si>
-  <si>
-    <t>https://gitlab.com/MHenderson1/notes/blob/master/11_12_08_constraint_psssodls.pdf</t>
   </si>
   <si>
     <t>http://bit.ly/2skFkut</t>
@@ -429,7 +429,32 @@
     <t>Code to accompany ALT 2005 paper.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://gitlab.com/MHenderson1/experts
+</t>
+  </si>
+  <si>
     <t>https://bitbucket.org/matthew/experts/src/default/</t>
+  </si>
+  <si>
+    <t>psssodls.py</t>
+  </si>
+  <si>
+    <t>Generator of PSSSODLS in Minion format.</t>
+  </si>
+  <si>
+    <t>https://gist.github.com/MHenderson/375a2122f1b77f90e5df</t>
+  </si>
+  <si>
+    <t>psssodls.eprime</t>
+  </si>
+  <si>
+    <t>Essence'</t>
+  </si>
+  <si>
+    <t>Essence' description of PSSSODLS</t>
+  </si>
+  <si>
+    <t>https://gist.github.com/MHenderson/6200476</t>
   </si>
 </sst>
 </file>
@@ -441,7 +466,7 @@
     <numFmt numFmtId="165" formatCode="mm/dd"/>
     <numFmt numFmtId="166" formatCode="m/d"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -453,11 +478,11 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <b/>
     </font>
     <font/>
     <font>
@@ -484,6 +509,10 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -499,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -507,24 +536,24 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -542,58 +571,71 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -725,7 +767,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L11" displayName="Table_4" id="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L13" displayName="Table_4" id="4">
   <tableColumns count="12">
     <tableColumn name="title" id="1"/>
     <tableColumn name="language" id="2"/>
@@ -956,42 +998,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D2" s="6">
         <v>7.0</v>
@@ -1009,84 +1051,84 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="14">
+      <c r="F3" s="15">
         <v>43475.0</v>
       </c>
       <c r="G3" s="6">
         <v>2009.0</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>32</v>
+      <c r="H3" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G4" s="6">
         <v>2009.0</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>46</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G5" s="6">
         <v>2005.0</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>32</v>
+      <c r="H5" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>55</v>
+      <c r="A6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="7"/>
@@ -1095,21 +1137,21 @@
       <c r="G6" s="6">
         <v>2005.0</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D7" s="6">
@@ -1124,11 +1166,11 @@
       <c r="G7" s="6">
         <v>2004.0</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>68</v>
+      <c r="H7" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1164,33 +1206,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="B2" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>22</v>
@@ -1199,101 +1241,101 @@
         <v>25</v>
       </c>
       <c r="E2" s="7"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>36</v>
-      </c>
       <c r="D3" s="12" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E3" s="7"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>49</v>
+      <c r="A4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E4" s="16">
         <v>43720.0</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>66</v>
+      <c r="A5" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E5" s="16">
         <v>43658.0</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>81</v>
       </c>
       <c r="E6" s="16">
         <v>43567.0</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="19">
         <v>43810.0</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
@@ -1308,11 +1350,11 @@
       <c r="D8" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="19">
         <v>43780.0</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
     </row>
     <row r="12">
       <c r="A12" s="24"/>
@@ -1361,27 +1403,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
+      <c r="A2" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
@@ -1394,7 +1436,7 @@
       <c r="F2" s="13"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1410,30 +1452,30 @@
       <c r="F3" s="13"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>40</v>
+      <c r="A4" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="18">
+        <v>43</v>
+      </c>
+      <c r="D4" s="19">
         <v>43782.0</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>51</v>
+      <c r="A5" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D5" s="16">
         <v>43721.0</v>
@@ -1442,14 +1484,14 @@
       <c r="F5" s="13"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>59</v>
+      <c r="A6" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D6" s="16">
         <v>43690.0</v>
@@ -1458,14 +1500,14 @@
       <c r="F6" s="13"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>71</v>
+      <c r="A7" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D7" s="16">
         <v>43659.0</v>
@@ -1474,14 +1516,14 @@
       <c r="F7" s="13"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>78</v>
+      <c r="A8" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D8" s="16">
         <v>43568.0</v>
@@ -1522,17 +1564,18 @@
     <col customWidth="1" min="3" max="3" width="31.71"/>
     <col customWidth="1" min="4" max="4" width="19.57"/>
     <col customWidth="1" min="5" max="5" width="17.0"/>
+    <col customWidth="1" min="6" max="6" width="18.71"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>90</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="25" t="s">
         <v>91</v>
@@ -1553,13 +1596,13 @@
         <v>96</v>
       </c>
       <c r="J1" s="25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K1" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="25" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="25" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2">
@@ -1569,7 +1612,7 @@
       <c r="B2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>99</v>
       </c>
       <c r="D2" s="12" t="s">
@@ -1595,7 +1638,7 @@
       <c r="B3" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>103</v>
       </c>
       <c r="D3" s="12" t="s">
@@ -1619,7 +1662,7 @@
       <c r="B4" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>108</v>
       </c>
       <c r="D4" s="12" t="s">
@@ -1643,7 +1686,7 @@
       <c r="B5" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>112</v>
       </c>
       <c r="D5" s="12" t="s">
@@ -1724,13 +1767,13 @@
       <c r="E8" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
@@ -1739,22 +1782,22 @@
       <c r="B9" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>128</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E9" s="30"/>
-      <c r="F9" s="15"/>
+      <c r="F9" s="14"/>
       <c r="G9" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
@@ -1763,7 +1806,7 @@
       <c r="B10" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>131</v>
       </c>
       <c r="D10" s="12" t="s">
@@ -1773,12 +1816,12 @@
       <c r="F10" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
@@ -1791,15 +1834,61 @@
         <v>135</v>
       </c>
       <c r="D11" s="31"/>
-      <c r="F11" s="15"/>
+      <c r="F11" s="12" t="s">
+        <v>136</v>
+      </c>
       <c r="G11" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
+        <v>137</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1822,11 +1911,15 @@
     <hyperlink r:id="rId17" ref="G9"/>
     <hyperlink r:id="rId18" ref="D10"/>
     <hyperlink r:id="rId19" ref="F10"/>
-    <hyperlink r:id="rId20" ref="G11"/>
+    <hyperlink r:id="rId20" ref="F11"/>
+    <hyperlink r:id="rId21" ref="G11"/>
+    <hyperlink r:id="rId22" ref="A12"/>
+    <hyperlink r:id="rId23" ref="E12"/>
+    <hyperlink r:id="rId24" ref="E13"/>
   </hyperlinks>
-  <drawing r:id="rId21"/>
+  <drawing r:id="rId25"/>
   <tableParts count="1">
-    <tablePart r:id="rId23"/>
+    <tablePart r:id="rId27"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>